<commit_message>
CAPM, FCF, and Brent Stuff
</commit_message>
<xml_diff>
--- a/BinomialPricingModel-Oil/InterestRates.xlsx
+++ b/BinomialPricingModel-Oil/InterestRates.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangkvi/Desktop/PythonFinanceShell/pyfi/BinomialPricingModel-Oil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EC0373E7-F232-9648-9DAD-847592B26C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C411E258-F5FA-0845-B603-5A75C8FE69C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16280" xr2:uid="{60191522-5B0D-E24A-87AF-1A4F7FD65336}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16280" activeTab="1" xr2:uid="{60191522-5B0D-E24A-87AF-1A4F7FD65336}"/>
   </bookViews>
   <sheets>
     <sheet name="ECB" sheetId="1" r:id="rId1"/>
-    <sheet name="FED" sheetId="2" r:id="rId2"/>
+    <sheet name="BrentOilPrices" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>FED</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -415,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5B08FF-870D-8B47-9FAF-31D7BB6A0C1E}">
   <dimension ref="A1:BJ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1187,12 +1190,519 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4DDFD9A-58FD-F147-BE1A-D3061A3803C3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>43830</v>
+      </c>
+      <c r="B2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43738</v>
+      </c>
+      <c r="B3">
+        <v>62.39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43646</v>
+      </c>
+      <c r="B4">
+        <v>65.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>43555</v>
+      </c>
+      <c r="B5">
+        <v>67.540000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43465</v>
+      </c>
+      <c r="B6">
+        <v>59.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43373</v>
+      </c>
+      <c r="B7">
+        <v>79.739999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>43281</v>
+      </c>
+      <c r="B8">
+        <v>76.459999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43190</v>
+      </c>
+      <c r="B9">
+        <v>69.53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43100</v>
+      </c>
+      <c r="B10">
+        <v>70.52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>43008</v>
+      </c>
+      <c r="B11">
+        <v>58.33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>42916</v>
+      </c>
+      <c r="B12">
+        <v>49.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>42825</v>
+      </c>
+      <c r="B13">
+        <v>55.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>42735</v>
+      </c>
+      <c r="B14">
+        <v>53.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>42643</v>
+      </c>
+      <c r="B15">
+        <v>50.61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>42551</v>
+      </c>
+      <c r="B16">
+        <v>45.26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>42460</v>
+      </c>
+      <c r="B17">
+        <v>42.86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>42369</v>
+      </c>
+      <c r="B18">
+        <v>33.58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>42277</v>
+      </c>
+      <c r="B19">
+        <v>48.23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>42185</v>
+      </c>
+      <c r="B20">
+        <v>56.52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>42094</v>
+      </c>
+      <c r="B21">
+        <v>62.84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>42004</v>
+      </c>
+      <c r="B22">
+        <v>51.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>41912</v>
+      </c>
+      <c r="B23">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>41820</v>
+      </c>
+      <c r="B24">
+        <v>107.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>41729</v>
+      </c>
+      <c r="B25">
+        <v>109.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>41639</v>
+      </c>
+      <c r="B26">
+        <v>106.31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>41547</v>
+      </c>
+      <c r="B27">
+        <v>111.21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>41455</v>
+      </c>
+      <c r="B28">
+        <v>107.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>41364</v>
+      </c>
+      <c r="B29">
+        <v>103.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>41274</v>
+      </c>
+      <c r="B30">
+        <v>113.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>41182</v>
+      </c>
+      <c r="B31">
+        <v>112.47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>41090</v>
+      </c>
+      <c r="B32">
+        <v>103.55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>40999</v>
+      </c>
+      <c r="B33">
+        <v>120.18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>40908</v>
+      </c>
+      <c r="B34">
+        <v>110.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>40816</v>
+      </c>
+      <c r="B35">
+        <v>111.45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>40724</v>
+      </c>
+      <c r="B36">
+        <v>118.15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>40633</v>
+      </c>
+      <c r="B37">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>40543</v>
+      </c>
+      <c r="B38">
+        <v>95.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>40451</v>
+      </c>
+      <c r="B39">
+        <v>79.03</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>40359</v>
+      </c>
+      <c r="B40">
+        <v>74.247</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>40268</v>
+      </c>
+      <c r="B41">
+        <v>81.17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>40178</v>
+      </c>
+      <c r="B42">
+        <v>72.989999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>40086</v>
+      </c>
+      <c r="B43">
+        <v>70.19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>39994</v>
+      </c>
+      <c r="B44">
+        <v>70.11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>39903</v>
+      </c>
+      <c r="B45">
+        <v>50.32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>39813</v>
+      </c>
+      <c r="B46">
+        <v>43.62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>39721</v>
+      </c>
+      <c r="B47">
+        <v>74.53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>39629</v>
+      </c>
+      <c r="B48">
+        <v>142.03</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>39538</v>
+      </c>
+      <c r="B49">
+        <v>111.36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>39447</v>
+      </c>
+      <c r="B50">
+        <v>89.07</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>39355</v>
+      </c>
+      <c r="B51">
+        <v>84.6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>39263</v>
+      </c>
+      <c r="B52">
+        <v>76.290000000000006</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>39172</v>
+      </c>
+      <c r="B53">
+        <v>67.84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>39082</v>
+      </c>
+      <c r="B54">
+        <v>53.68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>38990</v>
+      </c>
+      <c r="B55">
+        <v>59.21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>38898</v>
+      </c>
+      <c r="B56">
+        <v>76.28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>38807</v>
+      </c>
+      <c r="B57">
+        <v>69.41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>38717</v>
+      </c>
+      <c r="B58">
+        <v>66.150000000000006</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>38625</v>
+      </c>
+      <c r="B59">
+        <v>57.77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>38533</v>
+      </c>
+      <c r="B60">
+        <v>57.11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>38442</v>
+      </c>
+      <c r="B61">
+        <v>50.48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>38352</v>
+      </c>
+      <c r="B62">
+        <v>44.95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>38260</v>
+      </c>
+      <c r="B63">
+        <v>50.72</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finally finished the Financial Statements. Used Brent Futures and OCF to calculate net worth of future Shell projects
</commit_message>
<xml_diff>
--- a/BinomialPricingModel-Oil/InterestRates.xlsx
+++ b/BinomialPricingModel-Oil/InterestRates.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangkvi/Desktop/PythonFinanceShell/pyfi/BinomialPricingModel-Oil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C411E258-F5FA-0845-B603-5A75C8FE69C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DAE5EA-6201-6F4B-837E-4CD277D7BF2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16280" activeTab="1" xr2:uid="{60191522-5B0D-E24A-87AF-1A4F7FD65336}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="10120" windowHeight="16280" activeTab="2" xr2:uid="{60191522-5B0D-E24A-87AF-1A4F7FD65336}"/>
   </bookViews>
   <sheets>
     <sheet name="ECB" sheetId="1" r:id="rId1"/>
     <sheet name="BrentOilPrices" sheetId="2" r:id="rId2"/>
+    <sheet name="BrentFuture" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -44,6 +45,9 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>FuturePrice</t>
   </si>
 </sst>
 </file>
@@ -93,7 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -101,6 +105,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1192,7 +1197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4DDFD9A-58FD-F147-BE1A-D3061A3803C3}">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
@@ -1705,4 +1710,779 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DA3013-B4BF-0B42-863F-2BD892174520}">
+  <dimension ref="A1:B100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>43983</v>
+      </c>
+      <c r="B2">
+        <v>25.57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>44013</v>
+      </c>
+      <c r="B3">
+        <v>29.21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>44044</v>
+      </c>
+      <c r="B4">
+        <v>31.51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>44075</v>
+      </c>
+      <c r="B5">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>44105</v>
+      </c>
+      <c r="B6">
+        <v>34.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>44136</v>
+      </c>
+      <c r="B7">
+        <v>35.71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>44166</v>
+      </c>
+      <c r="B8">
+        <v>36.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>44197</v>
+      </c>
+      <c r="B9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>44228</v>
+      </c>
+      <c r="B10">
+        <v>37.549999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>44256</v>
+      </c>
+      <c r="B11">
+        <v>38.07</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>44287</v>
+      </c>
+      <c r="B12">
+        <v>38.450000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>44317</v>
+      </c>
+      <c r="B13">
+        <v>38.81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>44348</v>
+      </c>
+      <c r="B14">
+        <v>39.14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>44378</v>
+      </c>
+      <c r="B15">
+        <v>39.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>44409</v>
+      </c>
+      <c r="B16">
+        <v>39.69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>44440</v>
+      </c>
+      <c r="B17">
+        <v>39.979999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>44470</v>
+      </c>
+      <c r="B18">
+        <v>40.270000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>44501</v>
+      </c>
+      <c r="B19">
+        <v>40.56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>44531</v>
+      </c>
+      <c r="B20">
+        <v>40.86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>44562</v>
+      </c>
+      <c r="B21">
+        <v>41.12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>44593</v>
+      </c>
+      <c r="B22">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>44621</v>
+      </c>
+      <c r="B23">
+        <v>41.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>44652</v>
+      </c>
+      <c r="B24">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>44682</v>
+      </c>
+      <c r="B25">
+        <v>42.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>44713</v>
+      </c>
+      <c r="B26">
+        <v>42.59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>44743</v>
+      </c>
+      <c r="B27">
+        <v>42.81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>44774</v>
+      </c>
+      <c r="B28">
+        <v>43.03</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>44805</v>
+      </c>
+      <c r="B29">
+        <v>43.24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>44835</v>
+      </c>
+      <c r="B30">
+        <v>43.45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>44866</v>
+      </c>
+      <c r="B31">
+        <v>43.66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>44896</v>
+      </c>
+      <c r="B32">
+        <v>43.86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>44927</v>
+      </c>
+      <c r="B33">
+        <v>44.09</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>44958</v>
+      </c>
+      <c r="B34">
+        <v>44.33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>44986</v>
+      </c>
+      <c r="B35">
+        <v>44.57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>45017</v>
+      </c>
+      <c r="B36">
+        <v>44.82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
+        <v>45047</v>
+      </c>
+      <c r="B37">
+        <v>45.06</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
+        <v>45078</v>
+      </c>
+      <c r="B38">
+        <v>45.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
+        <v>45108</v>
+      </c>
+      <c r="B39">
+        <v>45.52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="7">
+        <v>45139</v>
+      </c>
+      <c r="B40">
+        <v>45.72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="7">
+        <v>45170</v>
+      </c>
+      <c r="B41">
+        <v>45.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
+        <v>45200</v>
+      </c>
+      <c r="B42">
+        <v>46.08</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="7">
+        <v>45231</v>
+      </c>
+      <c r="B43">
+        <v>46.26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
+        <v>45261</v>
+      </c>
+      <c r="B44">
+        <v>46.41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
+        <v>45292</v>
+      </c>
+      <c r="B45">
+        <v>46.63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
+        <v>45323</v>
+      </c>
+      <c r="B46">
+        <v>46.84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
+        <v>45352</v>
+      </c>
+      <c r="B47">
+        <v>47.04</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="7">
+        <v>45383</v>
+      </c>
+      <c r="B48">
+        <v>47.22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="7">
+        <v>45413</v>
+      </c>
+      <c r="B49">
+        <v>47.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="7">
+        <v>45444</v>
+      </c>
+      <c r="B50">
+        <v>47.58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="7">
+        <v>45474</v>
+      </c>
+      <c r="B51">
+        <v>47.76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="7">
+        <v>45505</v>
+      </c>
+      <c r="B52">
+        <v>47.94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="7">
+        <v>45536</v>
+      </c>
+      <c r="B53">
+        <v>48.12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="7">
+        <v>45566</v>
+      </c>
+      <c r="B54">
+        <v>48.3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="7">
+        <v>45597</v>
+      </c>
+      <c r="B55">
+        <v>48.48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="7">
+        <v>45627</v>
+      </c>
+      <c r="B56">
+        <v>48.65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="7">
+        <v>45658</v>
+      </c>
+      <c r="B57">
+        <v>48.83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="7">
+        <v>45689</v>
+      </c>
+      <c r="B58">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="7">
+        <v>45717</v>
+      </c>
+      <c r="B59">
+        <v>49.17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="7">
+        <v>45748</v>
+      </c>
+      <c r="B60">
+        <v>49.33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="7">
+        <v>45778</v>
+      </c>
+      <c r="B61">
+        <v>49.49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="7">
+        <v>45809</v>
+      </c>
+      <c r="B62">
+        <v>49.65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="7">
+        <v>45839</v>
+      </c>
+      <c r="B63">
+        <v>49.81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="7">
+        <v>45870</v>
+      </c>
+      <c r="B64">
+        <v>49.97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="7">
+        <v>45901</v>
+      </c>
+      <c r="B65">
+        <v>50.13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="7">
+        <v>45931</v>
+      </c>
+      <c r="B66">
+        <v>50.29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="7">
+        <v>45962</v>
+      </c>
+      <c r="B67">
+        <v>50.45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="7">
+        <v>45992</v>
+      </c>
+      <c r="B68">
+        <v>50.61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="7">
+        <v>46023</v>
+      </c>
+      <c r="B69">
+        <v>50.76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="7">
+        <v>46054</v>
+      </c>
+      <c r="B70">
+        <v>50.91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="7">
+        <v>46082</v>
+      </c>
+      <c r="B71">
+        <v>51.06</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="7">
+        <v>46113</v>
+      </c>
+      <c r="B72">
+        <v>51.21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="7">
+        <v>46143</v>
+      </c>
+      <c r="B73">
+        <v>51.38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="7">
+        <v>46174</v>
+      </c>
+      <c r="B74">
+        <v>51.55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="7">
+        <v>46204</v>
+      </c>
+      <c r="B75">
+        <v>51.72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="7">
+        <v>46235</v>
+      </c>
+      <c r="B76">
+        <v>51.89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="7">
+        <v>46266</v>
+      </c>
+      <c r="B77">
+        <v>52.06</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="7">
+        <v>46296</v>
+      </c>
+      <c r="B78">
+        <v>52.23</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="7">
+        <v>46327</v>
+      </c>
+      <c r="B79">
+        <v>52.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="7">
+        <v>46357</v>
+      </c>
+      <c r="B80">
+        <v>52.57</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="7">
+        <v>46388</v>
+      </c>
+      <c r="B81">
+        <v>52.63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="7">
+        <v>46419</v>
+      </c>
+      <c r="B82">
+        <v>52.69</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="7">
+        <v>46447</v>
+      </c>
+      <c r="B83">
+        <v>52.75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="7">
+        <v>46478</v>
+      </c>
+      <c r="B84">
+        <v>52.81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="7">
+        <v>46508</v>
+      </c>
+      <c r="B85">
+        <v>52.87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="7">
+        <v>46539</v>
+      </c>
+      <c r="B86">
+        <v>52.93</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="7">
+        <v>46569</v>
+      </c>
+      <c r="B87">
+        <v>52.99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="7">
+        <v>46600</v>
+      </c>
+      <c r="B88">
+        <v>53.05</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="7">
+        <v>46631</v>
+      </c>
+      <c r="B89">
+        <v>53.11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="7">
+        <v>46661</v>
+      </c>
+      <c r="B90">
+        <v>53.15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="7">
+        <v>46692</v>
+      </c>
+      <c r="B91">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="7">
+        <v>46722</v>
+      </c>
+      <c r="B92">
+        <v>53.25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="7"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="7"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="7"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="7"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="7"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="7"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="7"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>